<commit_message>
added grammar data to Spanish WS
</commit_message>
<xml_diff>
--- a/raw_data/Spanish_WS/[Spanish_WS].xlsx
+++ b/raw_data/Spanish_WS/[Spanish_WS].xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11611" uniqueCount="2360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11859" uniqueCount="2427">
   <si>
     <t>tutu</t>
   </si>
@@ -7101,13 +7101,214 @@
   </si>
   <si>
     <t>function_words</t>
+  </si>
+  <si>
+    <t>cmplx01</t>
+  </si>
+  <si>
+    <t>complexity</t>
+  </si>
+  <si>
+    <t>cmplx02</t>
+  </si>
+  <si>
+    <t>cmplx03</t>
+  </si>
+  <si>
+    <t>cmplx04</t>
+  </si>
+  <si>
+    <t>cmplx05</t>
+  </si>
+  <si>
+    <t>cmplx06</t>
+  </si>
+  <si>
+    <t>cmplx07</t>
+  </si>
+  <si>
+    <t>cmplx08</t>
+  </si>
+  <si>
+    <t>cmplx09</t>
+  </si>
+  <si>
+    <t>cmplx10</t>
+  </si>
+  <si>
+    <t>cmplx11</t>
+  </si>
+  <si>
+    <t>cmplx12</t>
+  </si>
+  <si>
+    <t>cmplx13</t>
+  </si>
+  <si>
+    <t>cmplx14</t>
+  </si>
+  <si>
+    <t>cmplx15</t>
+  </si>
+  <si>
+    <t>cmplx16</t>
+  </si>
+  <si>
+    <t>cmplx17</t>
+  </si>
+  <si>
+    <t>cmplx18</t>
+  </si>
+  <si>
+    <t>cmplx19</t>
+  </si>
+  <si>
+    <t>cmplx20</t>
+  </si>
+  <si>
+    <t>cmplx21</t>
+  </si>
+  <si>
+    <t>cmplx22</t>
+  </si>
+  <si>
+    <t>cmplx23</t>
+  </si>
+  <si>
+    <t>cmplx24</t>
+  </si>
+  <si>
+    <t>cmplx25</t>
+  </si>
+  <si>
+    <t>cmplx26</t>
+  </si>
+  <si>
+    <t>cmplx27</t>
+  </si>
+  <si>
+    <t>cmplx28</t>
+  </si>
+  <si>
+    <t>cmplx29</t>
+  </si>
+  <si>
+    <t>cmplx30</t>
+  </si>
+  <si>
+    <t>cmplx31</t>
+  </si>
+  <si>
+    <t>cmplx32</t>
+  </si>
+  <si>
+    <t>cmplx33</t>
+  </si>
+  <si>
+    <t>cmplx34</t>
+  </si>
+  <si>
+    <t>cmplx35</t>
+  </si>
+  <si>
+    <t>cmplx36</t>
+  </si>
+  <si>
+    <t>cmplx37</t>
+  </si>
+  <si>
+    <t>pracaba</t>
+  </si>
+  <si>
+    <t>word_form</t>
+  </si>
+  <si>
+    <t>pracabas</t>
+  </si>
+  <si>
+    <t>pracabms</t>
+  </si>
+  <si>
+    <t>pracabo</t>
+  </si>
+  <si>
+    <t>prcome</t>
+  </si>
+  <si>
+    <t>prcomems</t>
+  </si>
+  <si>
+    <t>prcomes</t>
+  </si>
+  <si>
+    <t>prcomo</t>
+  </si>
+  <si>
+    <t>prsube</t>
+  </si>
+  <si>
+    <t>prsubes</t>
+  </si>
+  <si>
+    <t>prsubims</t>
+  </si>
+  <si>
+    <t>prsubo</t>
+  </si>
+  <si>
+    <t>paacabe</t>
+  </si>
+  <si>
+    <t>paacabo</t>
+  </si>
+  <si>
+    <t>pacomi</t>
+  </si>
+  <si>
+    <t>pacomio</t>
+  </si>
+  <si>
+    <t>pasubi</t>
+  </si>
+  <si>
+    <t>pasubio</t>
+  </si>
+  <si>
+    <t>iacaba</t>
+  </si>
+  <si>
+    <t>iacabate</t>
+  </si>
+  <si>
+    <t>icome</t>
+  </si>
+  <si>
+    <t>icomete</t>
+  </si>
+  <si>
+    <t>isube</t>
+  </si>
+  <si>
+    <t>isubete</t>
+  </si>
+  <si>
+    <t>scombine</t>
+  </si>
+  <si>
+    <t>combine</t>
+  </si>
+  <si>
+    <t>simple, complex</t>
+  </si>
+  <si>
+    <t>yes, no</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7176,6 +7377,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -7209,7 +7416,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2046">
+  <cellStyleXfs count="2048">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9256,8 +9463,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9285,8 +9494,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2046">
+  <cellStyles count="2048">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -10309,6 +10520,7 @@
     <cellStyle name="Followed Hyperlink" xfId="2041" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2043" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2045" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2047" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -11331,6 +11543,7 @@
     <cellStyle name="Hyperlink" xfId="2040" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2042" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2044" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2046" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sheet1" xfId="1"/>
   </cellStyles>
@@ -11663,14 +11876,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H768"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A657" workbookViewId="0">
-      <selection activeCell="C633" sqref="C633"/>
+    <sheetView tabSelected="1" topLeftCell="A713" workbookViewId="0">
+      <selection activeCell="D741" sqref="D741"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
@@ -29384,356 +29598,914 @@
       </c>
     </row>
     <row r="682" spans="1:8">
-      <c r="A682" s="3"/>
-      <c r="B682" s="3"/>
-      <c r="C682" s="10"/>
+      <c r="A682" t="s">
+        <v>2360</v>
+      </c>
+      <c r="B682" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C682" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D682" t="s">
+        <v>2425</v>
+      </c>
     </row>
     <row r="683" spans="1:8">
-      <c r="A683" s="3"/>
-      <c r="B683" s="3"/>
-      <c r="C683" s="10"/>
+      <c r="A683" t="s">
+        <v>2362</v>
+      </c>
+      <c r="B683" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C683" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D683" t="s">
+        <v>2425</v>
+      </c>
     </row>
     <row r="684" spans="1:8">
-      <c r="A684" s="3"/>
-      <c r="B684" s="3"/>
-      <c r="C684" s="10"/>
+      <c r="A684" t="s">
+        <v>2363</v>
+      </c>
+      <c r="B684" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C684" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D684" t="s">
+        <v>2425</v>
+      </c>
     </row>
     <row r="685" spans="1:8">
-      <c r="A685" s="3"/>
-      <c r="B685" s="3"/>
-      <c r="C685" s="10"/>
+      <c r="A685" t="s">
+        <v>2364</v>
+      </c>
+      <c r="B685" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C685" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D685" t="s">
+        <v>2425</v>
+      </c>
     </row>
     <row r="686" spans="1:8">
-      <c r="A686" s="3"/>
-      <c r="B686" s="3"/>
-      <c r="C686" s="10"/>
+      <c r="A686" t="s">
+        <v>2365</v>
+      </c>
+      <c r="B686" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C686" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D686" t="s">
+        <v>2425</v>
+      </c>
     </row>
     <row r="687" spans="1:8">
-      <c r="A687" s="3"/>
-      <c r="B687" s="3"/>
-      <c r="C687" s="10"/>
+      <c r="A687" t="s">
+        <v>2366</v>
+      </c>
+      <c r="B687" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C687" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D687" t="s">
+        <v>2425</v>
+      </c>
     </row>
     <row r="688" spans="1:8">
-      <c r="A688" s="3"/>
-      <c r="B688" s="3"/>
-      <c r="C688" s="10"/>
-    </row>
-    <row r="689" spans="1:3">
-      <c r="A689" s="3"/>
-      <c r="B689" s="3"/>
-      <c r="C689" s="10"/>
-    </row>
-    <row r="690" spans="1:3">
-      <c r="A690" s="3"/>
-      <c r="B690" s="3"/>
-      <c r="C690" s="10"/>
-    </row>
-    <row r="691" spans="1:3">
-      <c r="A691" s="3"/>
-      <c r="B691" s="3"/>
-      <c r="C691" s="10"/>
-    </row>
-    <row r="692" spans="1:3">
-      <c r="A692" s="3"/>
-      <c r="B692" s="3"/>
-      <c r="C692" s="10"/>
-    </row>
-    <row r="693" spans="1:3">
-      <c r="A693" s="3"/>
-      <c r="B693" s="3"/>
-      <c r="C693" s="10"/>
-    </row>
-    <row r="694" spans="1:3">
-      <c r="A694" s="3"/>
-      <c r="B694" s="3"/>
-      <c r="C694" s="10"/>
-    </row>
-    <row r="695" spans="1:3">
-      <c r="A695" s="3"/>
-      <c r="B695" s="3"/>
-      <c r="C695" s="10"/>
-    </row>
-    <row r="696" spans="1:3">
-      <c r="A696" s="3"/>
-      <c r="B696" s="3"/>
-      <c r="C696" s="8"/>
-    </row>
-    <row r="697" spans="1:3">
-      <c r="A697" s="3"/>
-      <c r="B697" s="3"/>
-      <c r="C697" s="8"/>
-    </row>
-    <row r="698" spans="1:3">
-      <c r="A698" s="3"/>
-      <c r="B698" s="3"/>
-      <c r="C698" s="8"/>
-    </row>
-    <row r="699" spans="1:3">
-      <c r="A699" s="3"/>
-      <c r="B699" s="3"/>
-      <c r="C699" s="8"/>
-    </row>
-    <row r="700" spans="1:3">
-      <c r="A700" s="3"/>
-      <c r="B700" s="3"/>
-      <c r="C700" s="8"/>
-    </row>
-    <row r="701" spans="1:3">
-      <c r="A701" s="3"/>
-      <c r="B701" s="3"/>
-      <c r="C701" s="8"/>
-    </row>
-    <row r="702" spans="1:3">
-      <c r="A702" s="3"/>
-      <c r="B702" s="3"/>
-      <c r="C702" s="8"/>
-    </row>
-    <row r="703" spans="1:3">
-      <c r="A703" s="3"/>
-      <c r="B703" s="3"/>
-      <c r="C703" s="10"/>
-    </row>
-    <row r="704" spans="1:3">
-      <c r="A704" s="3"/>
-      <c r="B704" s="3"/>
-      <c r="C704" s="10"/>
-    </row>
-    <row r="705" spans="1:3">
-      <c r="A705" s="3"/>
-      <c r="B705" s="3"/>
-      <c r="C705" s="10"/>
-    </row>
-    <row r="706" spans="1:3">
-      <c r="A706" s="3"/>
-      <c r="B706" s="3"/>
-      <c r="C706" s="10"/>
-    </row>
-    <row r="707" spans="1:3">
-      <c r="A707" s="3"/>
-      <c r="B707" s="3"/>
-      <c r="C707" s="10"/>
-    </row>
-    <row r="708" spans="1:3">
-      <c r="A708" s="3"/>
-      <c r="B708" s="3"/>
-      <c r="C708" s="10"/>
-    </row>
-    <row r="709" spans="1:3">
-      <c r="A709" s="3"/>
-      <c r="B709" s="3"/>
-      <c r="C709" s="10"/>
-    </row>
-    <row r="710" spans="1:3">
-      <c r="A710" s="3"/>
-      <c r="B710" s="3"/>
-      <c r="C710" s="10"/>
-    </row>
-    <row r="711" spans="1:3">
-      <c r="A711" s="3"/>
-      <c r="B711" s="3"/>
-      <c r="C711" s="10"/>
-    </row>
-    <row r="712" spans="1:3">
-      <c r="A712" s="3"/>
-      <c r="B712" s="3"/>
-      <c r="C712" s="10"/>
-    </row>
-    <row r="713" spans="1:3">
-      <c r="A713" s="3"/>
-      <c r="B713" s="3"/>
-      <c r="C713" s="10"/>
-    </row>
-    <row r="714" spans="1:3">
-      <c r="A714" s="3"/>
-      <c r="B714" s="3"/>
-      <c r="C714" s="10"/>
-    </row>
-    <row r="715" spans="1:3">
-      <c r="A715" s="3"/>
-      <c r="B715" s="3"/>
-      <c r="C715" s="10"/>
-    </row>
-    <row r="716" spans="1:3">
-      <c r="A716" s="3"/>
-      <c r="B716" s="3"/>
-      <c r="C716" s="10"/>
-    </row>
-    <row r="717" spans="1:3">
-      <c r="A717" s="3"/>
-      <c r="B717" s="3"/>
-      <c r="C717" s="10"/>
-    </row>
-    <row r="718" spans="1:3">
-      <c r="A718" s="3"/>
-      <c r="B718" s="3"/>
-      <c r="C718" s="10"/>
-    </row>
-    <row r="719" spans="1:3">
-      <c r="A719" s="3"/>
-      <c r="B719" s="3"/>
-      <c r="C719" s="10"/>
-    </row>
-    <row r="720" spans="1:3">
-      <c r="A720" s="3"/>
-      <c r="B720" s="3"/>
-      <c r="C720" s="10"/>
-    </row>
-    <row r="721" spans="1:3">
-      <c r="A721" s="3"/>
-      <c r="B721" s="3"/>
-      <c r="C721" s="10"/>
-    </row>
-    <row r="722" spans="1:3">
-      <c r="A722" s="3"/>
-      <c r="B722" s="3"/>
-      <c r="C722" s="10"/>
-    </row>
-    <row r="723" spans="1:3">
-      <c r="A723" s="3"/>
-      <c r="B723" s="3"/>
-      <c r="C723" s="10"/>
-    </row>
-    <row r="724" spans="1:3">
-      <c r="A724" s="3"/>
-      <c r="B724" s="3"/>
-      <c r="C724" s="10"/>
-    </row>
-    <row r="725" spans="1:3">
-      <c r="A725" s="3"/>
-      <c r="B725" s="3"/>
-      <c r="C725" s="10"/>
-    </row>
-    <row r="726" spans="1:3">
-      <c r="A726" s="3"/>
-      <c r="B726" s="3"/>
-      <c r="C726" s="10"/>
-    </row>
-    <row r="727" spans="1:3">
-      <c r="A727" s="3"/>
-      <c r="B727" s="3"/>
-      <c r="C727" s="10"/>
-    </row>
-    <row r="728" spans="1:3">
-      <c r="A728" s="3"/>
-      <c r="B728" s="3"/>
-      <c r="C728" s="10"/>
-    </row>
-    <row r="729" spans="1:3">
-      <c r="A729" s="3"/>
-      <c r="B729" s="3"/>
-      <c r="C729" s="10"/>
-    </row>
-    <row r="730" spans="1:3">
-      <c r="A730" s="3"/>
-      <c r="B730" s="3"/>
-      <c r="C730" s="10"/>
-    </row>
-    <row r="731" spans="1:3">
-      <c r="A731" s="3"/>
-      <c r="B731" s="3"/>
-      <c r="C731" s="10"/>
-    </row>
-    <row r="732" spans="1:3">
-      <c r="A732" s="3"/>
-      <c r="B732" s="3"/>
-      <c r="C732" s="10"/>
-    </row>
-    <row r="733" spans="1:3">
-      <c r="A733" s="3"/>
-      <c r="B733" s="3"/>
-      <c r="C733" s="10"/>
-    </row>
-    <row r="734" spans="1:3">
-      <c r="A734" s="3"/>
-      <c r="B734" s="3"/>
-      <c r="C734" s="10"/>
-    </row>
-    <row r="735" spans="1:3">
-      <c r="A735" s="3"/>
-      <c r="B735" s="3"/>
-      <c r="C735" s="10"/>
-    </row>
-    <row r="736" spans="1:3">
-      <c r="A736" s="3"/>
-      <c r="B736" s="3"/>
-      <c r="C736" s="10"/>
-    </row>
-    <row r="737" spans="1:3">
-      <c r="A737" s="3"/>
-      <c r="B737" s="3"/>
-      <c r="C737" s="10"/>
-    </row>
-    <row r="738" spans="1:3">
-      <c r="A738" s="3"/>
-      <c r="B738" s="3"/>
-      <c r="C738" s="10"/>
-    </row>
-    <row r="739" spans="1:3">
-      <c r="A739" s="3"/>
-      <c r="B739" s="3"/>
-      <c r="C739" s="10"/>
-    </row>
-    <row r="740" spans="1:3">
-      <c r="A740" s="3"/>
-      <c r="B740" s="3"/>
-      <c r="C740" s="10"/>
-    </row>
-    <row r="741" spans="1:3">
-      <c r="A741" s="3"/>
-      <c r="B741" s="3"/>
-      <c r="C741" s="10"/>
-    </row>
-    <row r="742" spans="1:3">
-      <c r="A742" s="3"/>
-      <c r="B742" s="3"/>
-      <c r="C742" s="10"/>
-    </row>
-    <row r="743" spans="1:3">
-      <c r="A743" s="3"/>
-      <c r="B743" s="3"/>
-      <c r="C743" s="10"/>
-    </row>
-    <row r="744" spans="1:3">
+      <c r="A688" t="s">
+        <v>2367</v>
+      </c>
+      <c r="B688" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C688" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D688" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="689" spans="1:4">
+      <c r="A689" t="s">
+        <v>2368</v>
+      </c>
+      <c r="B689" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C689" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D689" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="690" spans="1:4">
+      <c r="A690" t="s">
+        <v>2369</v>
+      </c>
+      <c r="B690" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C690" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D690" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="691" spans="1:4">
+      <c r="A691" t="s">
+        <v>2370</v>
+      </c>
+      <c r="B691" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C691" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D691" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="692" spans="1:4">
+      <c r="A692" t="s">
+        <v>2371</v>
+      </c>
+      <c r="B692" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C692" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D692" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="693" spans="1:4">
+      <c r="A693" t="s">
+        <v>2372</v>
+      </c>
+      <c r="B693" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C693" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D693" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="694" spans="1:4">
+      <c r="A694" t="s">
+        <v>2373</v>
+      </c>
+      <c r="B694" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C694" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D694" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="695" spans="1:4">
+      <c r="A695" t="s">
+        <v>2374</v>
+      </c>
+      <c r="B695" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C695" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D695" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="696" spans="1:4">
+      <c r="A696" t="s">
+        <v>2375</v>
+      </c>
+      <c r="B696" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C696" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D696" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="697" spans="1:4">
+      <c r="A697" t="s">
+        <v>2376</v>
+      </c>
+      <c r="B697" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C697" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D697" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="698" spans="1:4">
+      <c r="A698" t="s">
+        <v>2377</v>
+      </c>
+      <c r="B698" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C698" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D698" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="699" spans="1:4">
+      <c r="A699" t="s">
+        <v>2378</v>
+      </c>
+      <c r="B699" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C699" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D699" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="700" spans="1:4">
+      <c r="A700" t="s">
+        <v>2379</v>
+      </c>
+      <c r="B700" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C700" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D700" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="701" spans="1:4">
+      <c r="A701" t="s">
+        <v>2380</v>
+      </c>
+      <c r="B701" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C701" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D701" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="702" spans="1:4">
+      <c r="A702" t="s">
+        <v>2381</v>
+      </c>
+      <c r="B702" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C702" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D702" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="703" spans="1:4">
+      <c r="A703" t="s">
+        <v>2382</v>
+      </c>
+      <c r="B703" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C703" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D703" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="704" spans="1:4">
+      <c r="A704" t="s">
+        <v>2383</v>
+      </c>
+      <c r="B704" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C704" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D704" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="705" spans="1:4">
+      <c r="A705" t="s">
+        <v>2384</v>
+      </c>
+      <c r="B705" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C705" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D705" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="706" spans="1:4">
+      <c r="A706" t="s">
+        <v>2385</v>
+      </c>
+      <c r="B706" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C706" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D706" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="707" spans="1:4">
+      <c r="A707" t="s">
+        <v>2386</v>
+      </c>
+      <c r="B707" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C707" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D707" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="708" spans="1:4">
+      <c r="A708" t="s">
+        <v>2387</v>
+      </c>
+      <c r="B708" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C708" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D708" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="709" spans="1:4">
+      <c r="A709" t="s">
+        <v>2388</v>
+      </c>
+      <c r="B709" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C709" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D709" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="710" spans="1:4">
+      <c r="A710" t="s">
+        <v>2389</v>
+      </c>
+      <c r="B710" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C710" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D710" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="711" spans="1:4">
+      <c r="A711" t="s">
+        <v>2390</v>
+      </c>
+      <c r="B711" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C711" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D711" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="712" spans="1:4">
+      <c r="A712" t="s">
+        <v>2391</v>
+      </c>
+      <c r="B712" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C712" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D712" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="713" spans="1:4">
+      <c r="A713" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B713" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C713" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D713" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="714" spans="1:4">
+      <c r="A714" t="s">
+        <v>2393</v>
+      </c>
+      <c r="B714" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C714" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D714" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="715" spans="1:4">
+      <c r="A715" t="s">
+        <v>2394</v>
+      </c>
+      <c r="B715" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C715" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D715" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="716" spans="1:4">
+      <c r="A716" t="s">
+        <v>2395</v>
+      </c>
+      <c r="B716" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C716" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D716" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="717" spans="1:4">
+      <c r="A717" t="s">
+        <v>2396</v>
+      </c>
+      <c r="B717" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C717" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D717" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="718" spans="1:4">
+      <c r="A718" t="s">
+        <v>2397</v>
+      </c>
+      <c r="B718" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C718" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D718" t="s">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="719" spans="1:4">
+      <c r="A719" t="s">
+        <v>2398</v>
+      </c>
+      <c r="B719" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C719" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D719" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="720" spans="1:4">
+      <c r="A720" t="s">
+        <v>2400</v>
+      </c>
+      <c r="B720" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C720" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D720" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="721" spans="1:4">
+      <c r="A721" t="s">
+        <v>2401</v>
+      </c>
+      <c r="B721" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C721" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D721" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="722" spans="1:4">
+      <c r="A722" t="s">
+        <v>2402</v>
+      </c>
+      <c r="B722" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C722" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D722" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="723" spans="1:4">
+      <c r="A723" t="s">
+        <v>2403</v>
+      </c>
+      <c r="B723" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C723" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D723" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="724" spans="1:4">
+      <c r="A724" t="s">
+        <v>2404</v>
+      </c>
+      <c r="B724" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C724" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D724" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="725" spans="1:4">
+      <c r="A725" t="s">
+        <v>2405</v>
+      </c>
+      <c r="B725" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C725" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D725" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="726" spans="1:4">
+      <c r="A726" t="s">
+        <v>2406</v>
+      </c>
+      <c r="B726" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C726" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D726" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="727" spans="1:4">
+      <c r="A727" t="s">
+        <v>2407</v>
+      </c>
+      <c r="B727" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C727" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D727" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="728" spans="1:4">
+      <c r="A728" t="s">
+        <v>2408</v>
+      </c>
+      <c r="B728" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C728" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D728" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="729" spans="1:4">
+      <c r="A729" t="s">
+        <v>2409</v>
+      </c>
+      <c r="B729" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C729" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D729" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="730" spans="1:4">
+      <c r="A730" t="s">
+        <v>2410</v>
+      </c>
+      <c r="B730" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C730" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D730" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="731" spans="1:4">
+      <c r="A731" t="s">
+        <v>2411</v>
+      </c>
+      <c r="B731" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C731" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D731" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="732" spans="1:4">
+      <c r="A732" t="s">
+        <v>2412</v>
+      </c>
+      <c r="B732" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C732" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D732" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="733" spans="1:4">
+      <c r="A733" t="s">
+        <v>2413</v>
+      </c>
+      <c r="B733" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C733" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D733" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="734" spans="1:4">
+      <c r="A734" t="s">
+        <v>2414</v>
+      </c>
+      <c r="B734" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C734" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D734" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="735" spans="1:4">
+      <c r="A735" t="s">
+        <v>2415</v>
+      </c>
+      <c r="B735" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C735" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D735" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="736" spans="1:4">
+      <c r="A736" t="s">
+        <v>2416</v>
+      </c>
+      <c r="B736" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C736" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D736" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="737" spans="1:4">
+      <c r="A737" t="s">
+        <v>2417</v>
+      </c>
+      <c r="B737" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C737" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D737" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="738" spans="1:4">
+      <c r="A738" t="s">
+        <v>2418</v>
+      </c>
+      <c r="B738" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C738" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D738" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="739" spans="1:4">
+      <c r="A739" t="s">
+        <v>2419</v>
+      </c>
+      <c r="B739" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C739" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D739" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="740" spans="1:4">
+      <c r="A740" t="s">
+        <v>2420</v>
+      </c>
+      <c r="B740" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C740" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D740" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="741" spans="1:4">
+      <c r="A741" t="s">
+        <v>2421</v>
+      </c>
+      <c r="B741" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C741" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D741" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="742" spans="1:4">
+      <c r="A742" t="s">
+        <v>2422</v>
+      </c>
+      <c r="B742" s="13" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C742" s="14" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D742" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="743" spans="1:4">
+      <c r="A743" t="s">
+        <v>2423</v>
+      </c>
+      <c r="B743" s="13" t="s">
+        <v>2424</v>
+      </c>
+      <c r="C743" s="14" t="s">
+        <v>2424</v>
+      </c>
+      <c r="D743" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="744" spans="1:4">
       <c r="A744" s="3"/>
       <c r="B744" s="3"/>
       <c r="C744" s="10"/>
     </row>
-    <row r="745" spans="1:3">
+    <row r="745" spans="1:4">
       <c r="A745" s="3"/>
       <c r="B745" s="3"/>
       <c r="C745" s="10"/>
     </row>
-    <row r="746" spans="1:3">
+    <row r="746" spans="1:4">
       <c r="A746" s="3"/>
       <c r="B746" s="3"/>
       <c r="C746" s="10"/>
     </row>
-    <row r="747" spans="1:3">
+    <row r="747" spans="1:4">
       <c r="A747" s="3"/>
       <c r="B747" s="3"/>
       <c r="C747" s="10"/>
     </row>
-    <row r="748" spans="1:3">
+    <row r="748" spans="1:4">
       <c r="A748" s="3"/>
       <c r="B748" s="3"/>
       <c r="C748" s="10"/>
     </row>
-    <row r="749" spans="1:3">
+    <row r="749" spans="1:4">
       <c r="A749" s="3"/>
       <c r="B749" s="3"/>
       <c r="C749" s="10"/>
     </row>
-    <row r="750" spans="1:3">
+    <row r="750" spans="1:4">
       <c r="A750" s="3"/>
       <c r="B750" s="3"/>
       <c r="C750" s="10"/>
     </row>
-    <row r="751" spans="1:3">
+    <row r="751" spans="1:4">
       <c r="A751" s="3"/>
       <c r="B751" s="3"/>
       <c r="C751" s="10"/>
     </row>
-    <row r="752" spans="1:3">
+    <row r="752" spans="1:4">
       <c r="A752" s="3"/>
       <c r="B752" s="3"/>
       <c r="C752" s="10"/>

</xml_diff>

<commit_message>
item definitions for grammar items
</commit_message>
<xml_diff>
--- a/raw_data/Spanish_WS/[Spanish_WS].xlsx
+++ b/raw_data/Spanish_WS/[Spanish_WS].xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11859" uniqueCount="2427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11945" uniqueCount="2501">
   <si>
     <t>tutu</t>
   </si>
@@ -7302,6 +7302,228 @@
   </si>
   <si>
     <t>yes, no</t>
+  </si>
+  <si>
+    <t>usepast</t>
+  </si>
+  <si>
+    <t>usage</t>
+  </si>
+  <si>
+    <t>how_use_words</t>
+  </si>
+  <si>
+    <t>not yet, sometimes, often</t>
+  </si>
+  <si>
+    <t>does your child ever talk about past events or people who are not present?</t>
+  </si>
+  <si>
+    <t>usefuture</t>
+  </si>
+  <si>
+    <t>does your child ever talk about something that's going to happen in the future?</t>
+  </si>
+  <si>
+    <t>miss_produce</t>
+  </si>
+  <si>
+    <t>does your child talk a bout objects that are not present?</t>
+  </si>
+  <si>
+    <t>miss_comp</t>
+  </si>
+  <si>
+    <t>does your child understand if you ask for something that is not in the room?</t>
+  </si>
+  <si>
+    <t>usepossessive</t>
+  </si>
+  <si>
+    <t>does your child ever pick up or point to an object and name an absent person to whom the object belongs?</t>
+  </si>
+  <si>
+    <t>acaba (present)</t>
+  </si>
+  <si>
+    <t>acabas (present)</t>
+  </si>
+  <si>
+    <t>acabamos (present)</t>
+  </si>
+  <si>
+    <t>acabo (present)</t>
+  </si>
+  <si>
+    <t>come (present)</t>
+  </si>
+  <si>
+    <t>comemos (present)</t>
+  </si>
+  <si>
+    <t>comes (present)</t>
+  </si>
+  <si>
+    <t>como (present)</t>
+  </si>
+  <si>
+    <t>sube (present)</t>
+  </si>
+  <si>
+    <t>subes (present)</t>
+  </si>
+  <si>
+    <t>subo (present)</t>
+  </si>
+  <si>
+    <t>subimos (present)</t>
+  </si>
+  <si>
+    <t>acaba (imperative)</t>
+  </si>
+  <si>
+    <t>come (imperative)</t>
+  </si>
+  <si>
+    <t>sube (imperative)</t>
+  </si>
+  <si>
+    <t>acabé (past)</t>
+  </si>
+  <si>
+    <t>acabó (past)</t>
+  </si>
+  <si>
+    <t>comió (past)</t>
+  </si>
+  <si>
+    <t>subió (past)</t>
+  </si>
+  <si>
+    <t>comí (past)</t>
+  </si>
+  <si>
+    <t>subí (past)</t>
+  </si>
+  <si>
+    <t>acábate (imperative)</t>
+  </si>
+  <si>
+    <t>cómete (imperative)</t>
+  </si>
+  <si>
+    <t>súbete (imperative)</t>
+  </si>
+  <si>
+    <t>nene quiere / quiro paleta</t>
+  </si>
+  <si>
+    <t>tuyo esto / este es tuyo</t>
+  </si>
+  <si>
+    <t>Tito malo / soy malo</t>
+  </si>
+  <si>
+    <t>Pepe uvas / quiero uvas</t>
+  </si>
+  <si>
+    <t>agua vamos / vamos al agua</t>
+  </si>
+  <si>
+    <t>a silla / en la silla</t>
+  </si>
+  <si>
+    <t>pollo no / no quiero pollo</t>
+  </si>
+  <si>
+    <t>Paloma llorando / Paloma está llorando</t>
+  </si>
+  <si>
+    <t>mío lápiz / éste es mi lápiz</t>
+  </si>
+  <si>
+    <t>más leche / dame más leche</t>
+  </si>
+  <si>
+    <t>papo mami / el zapato es de mami</t>
+  </si>
+  <si>
+    <t>no aquí / ése no está aquí</t>
+  </si>
+  <si>
+    <t>rompió globo / se rompió el globo</t>
+  </si>
+  <si>
+    <t>leche caliente / la leche está caliente</t>
+  </si>
+  <si>
+    <t>duele panza / me duele la panza</t>
+  </si>
+  <si>
+    <t>guaguá grande / tengo un perro grande</t>
+  </si>
+  <si>
+    <t>calle allá está / allá está la calle</t>
+  </si>
+  <si>
+    <t>puse a mano / lo puse en mi mano</t>
+  </si>
+  <si>
+    <t>acabó agua / se me acabó agua</t>
+  </si>
+  <si>
+    <t>fue casa / se fue a su casa</t>
+  </si>
+  <si>
+    <t>silla subir / me quiero subir a la silla</t>
+  </si>
+  <si>
+    <t>Marta papá / quiero ir con papá</t>
+  </si>
+  <si>
+    <t>bravo Tello circo / dije bravo en el circo</t>
+  </si>
+  <si>
+    <t>papá calle / papá se fue a trabajar</t>
+  </si>
+  <si>
+    <t>ya puse / ya se lo puse</t>
+  </si>
+  <si>
+    <t>Chalo osito coche / Chalo dejó el osito en el coche</t>
+  </si>
+  <si>
+    <t>lápiz dibujar / dibujo con el lápiz</t>
+  </si>
+  <si>
+    <t>ya pinté / ya acabé de pintar</t>
+  </si>
+  <si>
+    <t>nene rompió bici Danny / el niño rompió la bici de Danny</t>
+  </si>
+  <si>
+    <t>pone no / no lo pongas</t>
+  </si>
+  <si>
+    <t>vamos comer papas carne / vamos a comer papas y carne</t>
+  </si>
+  <si>
+    <t>niño llora cayó / el niño llora porque se cayó</t>
+  </si>
+  <si>
+    <t>mamá nene compra / mamá y nene fueron a comprar</t>
+  </si>
+  <si>
+    <t>abre dame galleta / abre la caja y dame una galleta</t>
+  </si>
+  <si>
+    <t>no toca, quemas / no lo toques porque te quemas</t>
+  </si>
+  <si>
+    <t>quiero libro papá / quiero el libra que compró papá</t>
+  </si>
+  <si>
+    <t>pongo agua flores / pongo agua para que crezcan las flores</t>
   </si>
 </sst>
 </file>
@@ -7392,7 +7614,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -7415,8 +7637,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2048">
+  <cellStyleXfs count="2054">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9465,8 +9707,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9496,8 +9744,22 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2048">
+  <cellStyles count="2054">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -10521,6 +10783,9 @@
     <cellStyle name="Followed Hyperlink" xfId="2043" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2045" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2047" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2049" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2051" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2053" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -11544,6 +11809,9 @@
     <cellStyle name="Hyperlink" xfId="2042" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2044" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2046" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2048" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2050" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2052" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sheet1" xfId="1"/>
   </cellStyles>
@@ -11874,20 +12142,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H768"/>
+  <dimension ref="A1:H748"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A713" workbookViewId="0">
-      <selection activeCell="D741" sqref="D741"/>
+    <sheetView tabSelected="1" topLeftCell="A687" workbookViewId="0">
+      <selection activeCell="G731" sqref="G731"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -29597,429 +29866,526 @@
         <v>2359</v>
       </c>
     </row>
-    <row r="682" spans="1:8">
-      <c r="A682" t="s">
-        <v>2360</v>
-      </c>
-      <c r="B682" s="13" t="s">
-        <v>2361</v>
-      </c>
-      <c r="C682" s="14" t="s">
-        <v>2361</v>
-      </c>
-      <c r="D682" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="683" spans="1:8">
-      <c r="A683" t="s">
-        <v>2362</v>
-      </c>
-      <c r="B683" s="13" t="s">
-        <v>2361</v>
-      </c>
-      <c r="C683" s="14" t="s">
-        <v>2361</v>
-      </c>
-      <c r="D683" t="s">
-        <v>2425</v>
+    <row r="682" spans="1:8" ht="28">
+      <c r="A682" s="15" t="s">
+        <v>2427</v>
+      </c>
+      <c r="B682" s="16" t="s">
+        <v>2428</v>
+      </c>
+      <c r="C682" s="17" t="s">
+        <v>2429</v>
+      </c>
+      <c r="D682" s="2" t="s">
+        <v>2430</v>
+      </c>
+      <c r="E682" s="2"/>
+      <c r="F682" s="18"/>
+      <c r="G682" s="18" t="s">
+        <v>2431</v>
+      </c>
+    </row>
+    <row r="683" spans="1:8" ht="28">
+      <c r="A683" s="15" t="s">
+        <v>2432</v>
+      </c>
+      <c r="B683" s="16" t="s">
+        <v>2428</v>
+      </c>
+      <c r="C683" s="17" t="s">
+        <v>2429</v>
+      </c>
+      <c r="D683" s="2" t="s">
+        <v>2430</v>
+      </c>
+      <c r="E683" s="2"/>
+      <c r="F683" s="18"/>
+      <c r="G683" s="18" t="s">
+        <v>2433</v>
       </c>
     </row>
     <row r="684" spans="1:8">
-      <c r="A684" t="s">
-        <v>2363</v>
-      </c>
-      <c r="B684" s="13" t="s">
-        <v>2361</v>
-      </c>
-      <c r="C684" s="14" t="s">
-        <v>2361</v>
-      </c>
-      <c r="D684" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="685" spans="1:8">
-      <c r="A685" t="s">
-        <v>2364</v>
-      </c>
-      <c r="B685" s="13" t="s">
-        <v>2361</v>
-      </c>
-      <c r="C685" s="14" t="s">
-        <v>2361</v>
-      </c>
-      <c r="D685" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="686" spans="1:8">
-      <c r="A686" t="s">
-        <v>2365</v>
-      </c>
-      <c r="B686" s="13" t="s">
-        <v>2361</v>
-      </c>
-      <c r="C686" s="14" t="s">
-        <v>2361</v>
-      </c>
-      <c r="D686" t="s">
-        <v>2425</v>
+      <c r="A684" s="15" t="s">
+        <v>2434</v>
+      </c>
+      <c r="B684" s="16" t="s">
+        <v>2428</v>
+      </c>
+      <c r="C684" s="17" t="s">
+        <v>2429</v>
+      </c>
+      <c r="D684" s="2" t="s">
+        <v>2430</v>
+      </c>
+      <c r="E684" s="2"/>
+      <c r="F684" s="18"/>
+      <c r="G684" s="18" t="s">
+        <v>2435</v>
+      </c>
+    </row>
+    <row r="685" spans="1:8" ht="28">
+      <c r="A685" s="15" t="s">
+        <v>2436</v>
+      </c>
+      <c r="B685" s="16" t="s">
+        <v>2428</v>
+      </c>
+      <c r="C685" s="17" t="s">
+        <v>2429</v>
+      </c>
+      <c r="D685" s="2" t="s">
+        <v>2430</v>
+      </c>
+      <c r="E685" s="2"/>
+      <c r="F685" s="18"/>
+      <c r="G685" s="18" t="s">
+        <v>2437</v>
+      </c>
+    </row>
+    <row r="686" spans="1:8" ht="28">
+      <c r="A686" s="15" t="s">
+        <v>2438</v>
+      </c>
+      <c r="B686" s="16" t="s">
+        <v>2428</v>
+      </c>
+      <c r="C686" s="17" t="s">
+        <v>2429</v>
+      </c>
+      <c r="D686" s="2" t="s">
+        <v>2430</v>
+      </c>
+      <c r="E686" s="2"/>
+      <c r="F686" s="18"/>
+      <c r="G686" s="18" t="s">
+        <v>2439</v>
       </c>
     </row>
     <row r="687" spans="1:8">
       <c r="A687" t="s">
-        <v>2366</v>
+        <v>2398</v>
       </c>
       <c r="B687" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C687" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D687" t="s">
-        <v>2425</v>
+        <v>2331</v>
+      </c>
+      <c r="G687" s="19" t="s">
+        <v>2440</v>
       </c>
     </row>
     <row r="688" spans="1:8">
       <c r="A688" t="s">
-        <v>2367</v>
+        <v>2400</v>
       </c>
       <c r="B688" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C688" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D688" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="689" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G688" t="s">
+        <v>2441</v>
+      </c>
+    </row>
+    <row r="689" spans="1:7">
       <c r="A689" t="s">
-        <v>2368</v>
+        <v>2401</v>
       </c>
       <c r="B689" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C689" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D689" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="690" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G689" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="690" spans="1:7">
       <c r="A690" t="s">
-        <v>2369</v>
+        <v>2402</v>
       </c>
       <c r="B690" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C690" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D690" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="691" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G690" t="s">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="691" spans="1:7">
       <c r="A691" t="s">
-        <v>2370</v>
+        <v>2403</v>
       </c>
       <c r="B691" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C691" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D691" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="692" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G691" t="s">
+        <v>2444</v>
+      </c>
+    </row>
+    <row r="692" spans="1:7">
       <c r="A692" t="s">
-        <v>2371</v>
+        <v>2404</v>
       </c>
       <c r="B692" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C692" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D692" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="693" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G692" t="s">
+        <v>2445</v>
+      </c>
+    </row>
+    <row r="693" spans="1:7">
       <c r="A693" t="s">
-        <v>2372</v>
+        <v>2405</v>
       </c>
       <c r="B693" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C693" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D693" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="694" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G693" t="s">
+        <v>2446</v>
+      </c>
+    </row>
+    <row r="694" spans="1:7">
       <c r="A694" t="s">
-        <v>2373</v>
+        <v>2406</v>
       </c>
       <c r="B694" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C694" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D694" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="695" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G694" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="695" spans="1:7">
       <c r="A695" t="s">
-        <v>2374</v>
+        <v>2407</v>
       </c>
       <c r="B695" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C695" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D695" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="696" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G695" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="696" spans="1:7">
       <c r="A696" t="s">
-        <v>2375</v>
+        <v>2408</v>
       </c>
       <c r="B696" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C696" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D696" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="697" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G696" t="s">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="697" spans="1:7">
       <c r="A697" t="s">
-        <v>2376</v>
+        <v>2409</v>
       </c>
       <c r="B697" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C697" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D697" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="698" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G697" t="s">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="698" spans="1:7">
       <c r="A698" t="s">
-        <v>2377</v>
+        <v>2410</v>
       </c>
       <c r="B698" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C698" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D698" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="699" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G698" t="s">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="699" spans="1:7">
       <c r="A699" t="s">
-        <v>2378</v>
+        <v>2411</v>
       </c>
       <c r="B699" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C699" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D699" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="700" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G699" s="20" t="s">
+        <v>2455</v>
+      </c>
+    </row>
+    <row r="700" spans="1:7">
       <c r="A700" t="s">
-        <v>2379</v>
+        <v>2412</v>
       </c>
       <c r="B700" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C700" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D700" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="701" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G700" t="s">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="701" spans="1:7">
       <c r="A701" t="s">
-        <v>2380</v>
+        <v>2413</v>
       </c>
       <c r="B701" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C701" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D701" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="702" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G701" t="s">
+        <v>2459</v>
+      </c>
+    </row>
+    <row r="702" spans="1:7">
       <c r="A702" t="s">
-        <v>2381</v>
+        <v>2414</v>
       </c>
       <c r="B702" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C702" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D702" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="703" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G702" t="s">
+        <v>2457</v>
+      </c>
+    </row>
+    <row r="703" spans="1:7">
       <c r="A703" t="s">
-        <v>2382</v>
+        <v>2415</v>
       </c>
       <c r="B703" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C703" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D703" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="704" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G703" t="s">
+        <v>2460</v>
+      </c>
+    </row>
+    <row r="704" spans="1:7">
       <c r="A704" t="s">
-        <v>2383</v>
+        <v>2416</v>
       </c>
       <c r="B704" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C704" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D704" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="705" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G704" t="s">
+        <v>2458</v>
+      </c>
+    </row>
+    <row r="705" spans="1:7">
       <c r="A705" t="s">
-        <v>2384</v>
+        <v>2417</v>
       </c>
       <c r="B705" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C705" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D705" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="706" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G705" t="s">
+        <v>2452</v>
+      </c>
+    </row>
+    <row r="706" spans="1:7">
       <c r="A706" t="s">
-        <v>2385</v>
+        <v>2418</v>
       </c>
       <c r="B706" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C706" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D706" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="707" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G706" t="s">
+        <v>2461</v>
+      </c>
+    </row>
+    <row r="707" spans="1:7">
       <c r="A707" t="s">
-        <v>2386</v>
+        <v>2419</v>
       </c>
       <c r="B707" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C707" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D707" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="708" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G707" t="s">
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="708" spans="1:7">
       <c r="A708" t="s">
-        <v>2387</v>
+        <v>2420</v>
       </c>
       <c r="B708" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C708" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D708" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="709" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G708" t="s">
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="709" spans="1:7">
       <c r="A709" t="s">
-        <v>2388</v>
+        <v>2421</v>
       </c>
       <c r="B709" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C709" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D709" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="710" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G709" t="s">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="710" spans="1:7">
       <c r="A710" t="s">
-        <v>2389</v>
+        <v>2422</v>
       </c>
       <c r="B710" s="13" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="C710" s="14" t="s">
-        <v>2361</v>
+        <v>2399</v>
       </c>
       <c r="D710" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="711" spans="1:4">
+        <v>2331</v>
+      </c>
+      <c r="G710" t="s">
+        <v>2463</v>
+      </c>
+    </row>
+    <row r="711" spans="1:7">
       <c r="A711" t="s">
-        <v>2390</v>
+        <v>2423</v>
       </c>
       <c r="B711" s="13" t="s">
-        <v>2361</v>
+        <v>2424</v>
       </c>
       <c r="C711" s="14" t="s">
-        <v>2361</v>
+        <v>2424</v>
       </c>
       <c r="D711" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="712" spans="1:4">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="712" spans="1:7">
       <c r="A712" t="s">
-        <v>2391</v>
+        <v>2360</v>
       </c>
       <c r="B712" s="13" t="s">
         <v>2361</v>
@@ -30030,10 +30396,13 @@
       <c r="D712" t="s">
         <v>2425</v>
       </c>
-    </row>
-    <row r="713" spans="1:4">
+      <c r="G712" t="s">
+        <v>2464</v>
+      </c>
+    </row>
+    <row r="713" spans="1:7">
       <c r="A713" t="s">
-        <v>2392</v>
+        <v>2362</v>
       </c>
       <c r="B713" s="13" t="s">
         <v>2361</v>
@@ -30044,10 +30413,13 @@
       <c r="D713" t="s">
         <v>2425</v>
       </c>
-    </row>
-    <row r="714" spans="1:4">
+      <c r="G713" t="s">
+        <v>2465</v>
+      </c>
+    </row>
+    <row r="714" spans="1:7">
       <c r="A714" t="s">
-        <v>2393</v>
+        <v>2363</v>
       </c>
       <c r="B714" s="13" t="s">
         <v>2361</v>
@@ -30058,10 +30430,13 @@
       <c r="D714" t="s">
         <v>2425</v>
       </c>
-    </row>
-    <row r="715" spans="1:4">
+      <c r="G714" t="s">
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="715" spans="1:7">
       <c r="A715" t="s">
-        <v>2394</v>
+        <v>2364</v>
       </c>
       <c r="B715" s="13" t="s">
         <v>2361</v>
@@ -30072,10 +30447,13 @@
       <c r="D715" t="s">
         <v>2425</v>
       </c>
-    </row>
-    <row r="716" spans="1:4">
+      <c r="G715" t="s">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="716" spans="1:7">
       <c r="A716" t="s">
-        <v>2395</v>
+        <v>2365</v>
       </c>
       <c r="B716" s="13" t="s">
         <v>2361</v>
@@ -30086,10 +30464,13 @@
       <c r="D716" t="s">
         <v>2425</v>
       </c>
-    </row>
-    <row r="717" spans="1:4">
+      <c r="G716" t="s">
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="717" spans="1:7">
       <c r="A717" t="s">
-        <v>2396</v>
+        <v>2366</v>
       </c>
       <c r="B717" s="13" t="s">
         <v>2361</v>
@@ -30100,10 +30481,13 @@
       <c r="D717" t="s">
         <v>2425</v>
       </c>
-    </row>
-    <row r="718" spans="1:4">
+      <c r="G717" t="s">
+        <v>2469</v>
+      </c>
+    </row>
+    <row r="718" spans="1:7">
       <c r="A718" t="s">
-        <v>2397</v>
+        <v>2367</v>
       </c>
       <c r="B718" s="13" t="s">
         <v>2361</v>
@@ -30114,477 +30498,519 @@
       <c r="D718" t="s">
         <v>2425</v>
       </c>
-    </row>
-    <row r="719" spans="1:4">
+      <c r="G718" t="s">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="719" spans="1:7">
       <c r="A719" t="s">
-        <v>2398</v>
+        <v>2368</v>
       </c>
       <c r="B719" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C719" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D719" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="720" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G719" t="s">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="720" spans="1:7">
       <c r="A720" t="s">
-        <v>2400</v>
+        <v>2369</v>
       </c>
       <c r="B720" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C720" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D720" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="721" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G720" t="s">
+        <v>2472</v>
+      </c>
+    </row>
+    <row r="721" spans="1:7">
       <c r="A721" t="s">
-        <v>2401</v>
+        <v>2370</v>
       </c>
       <c r="B721" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C721" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D721" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="722" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G721" t="s">
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="722" spans="1:7">
       <c r="A722" t="s">
-        <v>2402</v>
+        <v>2371</v>
       </c>
       <c r="B722" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C722" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D722" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="723" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G722" t="s">
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="723" spans="1:7">
       <c r="A723" t="s">
-        <v>2403</v>
+        <v>2372</v>
       </c>
       <c r="B723" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C723" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D723" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="724" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G723" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="724" spans="1:7">
       <c r="A724" t="s">
-        <v>2404</v>
+        <v>2373</v>
       </c>
       <c r="B724" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C724" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D724" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="725" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G724" t="s">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="725" spans="1:7">
       <c r="A725" t="s">
-        <v>2405</v>
+        <v>2374</v>
       </c>
       <c r="B725" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C725" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D725" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="726" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G725" t="s">
+        <v>2477</v>
+      </c>
+    </row>
+    <row r="726" spans="1:7">
       <c r="A726" t="s">
-        <v>2406</v>
+        <v>2375</v>
       </c>
       <c r="B726" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C726" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D726" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="727" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G726" t="s">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="727" spans="1:7">
       <c r="A727" t="s">
-        <v>2407</v>
+        <v>2376</v>
       </c>
       <c r="B727" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C727" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D727" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="728" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G727" t="s">
+        <v>2479</v>
+      </c>
+    </row>
+    <row r="728" spans="1:7">
       <c r="A728" t="s">
-        <v>2408</v>
+        <v>2377</v>
       </c>
       <c r="B728" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C728" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D728" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="729" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G728" t="s">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="729" spans="1:7">
       <c r="A729" t="s">
-        <v>2409</v>
+        <v>2378</v>
       </c>
       <c r="B729" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C729" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D729" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="730" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G729" t="s">
+        <v>2481</v>
+      </c>
+    </row>
+    <row r="730" spans="1:7">
       <c r="A730" t="s">
-        <v>2410</v>
+        <v>2379</v>
       </c>
       <c r="B730" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C730" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D730" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="731" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G730" t="s">
+        <v>2482</v>
+      </c>
+    </row>
+    <row r="731" spans="1:7">
       <c r="A731" t="s">
-        <v>2411</v>
+        <v>2380</v>
       </c>
       <c r="B731" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C731" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D731" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="732" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G731" t="s">
+        <v>2483</v>
+      </c>
+    </row>
+    <row r="732" spans="1:7">
       <c r="A732" t="s">
-        <v>2412</v>
+        <v>2381</v>
       </c>
       <c r="B732" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C732" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D732" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="733" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G732" t="s">
+        <v>2484</v>
+      </c>
+    </row>
+    <row r="733" spans="1:7">
       <c r="A733" t="s">
-        <v>2413</v>
+        <v>2382</v>
       </c>
       <c r="B733" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C733" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D733" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="734" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G733" t="s">
+        <v>2485</v>
+      </c>
+    </row>
+    <row r="734" spans="1:7">
       <c r="A734" t="s">
-        <v>2414</v>
+        <v>2383</v>
       </c>
       <c r="B734" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C734" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D734" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="735" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G734" t="s">
+        <v>2486</v>
+      </c>
+    </row>
+    <row r="735" spans="1:7">
       <c r="A735" t="s">
-        <v>2415</v>
+        <v>2384</v>
       </c>
       <c r="B735" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C735" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D735" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="736" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G735" t="s">
+        <v>2487</v>
+      </c>
+    </row>
+    <row r="736" spans="1:7">
       <c r="A736" t="s">
-        <v>2416</v>
+        <v>2385</v>
       </c>
       <c r="B736" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C736" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D736" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="737" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G736" t="s">
+        <v>2488</v>
+      </c>
+    </row>
+    <row r="737" spans="1:7">
       <c r="A737" t="s">
-        <v>2417</v>
+        <v>2386</v>
       </c>
       <c r="B737" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C737" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D737" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="738" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G737" t="s">
+        <v>2489</v>
+      </c>
+    </row>
+    <row r="738" spans="1:7">
       <c r="A738" t="s">
-        <v>2418</v>
+        <v>2387</v>
       </c>
       <c r="B738" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C738" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D738" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="739" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G738" t="s">
+        <v>2490</v>
+      </c>
+    </row>
+    <row r="739" spans="1:7">
       <c r="A739" t="s">
-        <v>2419</v>
+        <v>2388</v>
       </c>
       <c r="B739" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C739" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D739" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="740" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G739" t="s">
+        <v>2491</v>
+      </c>
+    </row>
+    <row r="740" spans="1:7">
       <c r="A740" t="s">
-        <v>2420</v>
+        <v>2389</v>
       </c>
       <c r="B740" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C740" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D740" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="741" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G740" t="s">
+        <v>2492</v>
+      </c>
+    </row>
+    <row r="741" spans="1:7">
       <c r="A741" t="s">
-        <v>2421</v>
+        <v>2390</v>
       </c>
       <c r="B741" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C741" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D741" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="742" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G741" t="s">
+        <v>2493</v>
+      </c>
+    </row>
+    <row r="742" spans="1:7">
       <c r="A742" t="s">
-        <v>2422</v>
+        <v>2391</v>
       </c>
       <c r="B742" s="13" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="C742" s="14" t="s">
-        <v>2399</v>
+        <v>2361</v>
       </c>
       <c r="D742" t="s">
-        <v>2331</v>
-      </c>
-    </row>
-    <row r="743" spans="1:4">
+        <v>2425</v>
+      </c>
+      <c r="G742" t="s">
+        <v>2494</v>
+      </c>
+    </row>
+    <row r="743" spans="1:7">
       <c r="A743" t="s">
-        <v>2423</v>
+        <v>2392</v>
       </c>
       <c r="B743" s="13" t="s">
-        <v>2424</v>
+        <v>2361</v>
       </c>
       <c r="C743" s="14" t="s">
-        <v>2424</v>
+        <v>2361</v>
       </c>
       <c r="D743" t="s">
-        <v>2426</v>
-      </c>
-    </row>
-    <row r="744" spans="1:4">
-      <c r="A744" s="3"/>
-      <c r="B744" s="3"/>
-      <c r="C744" s="10"/>
-    </row>
-    <row r="745" spans="1:4">
-      <c r="A745" s="3"/>
-      <c r="B745" s="3"/>
-      <c r="C745" s="10"/>
-    </row>
-    <row r="746" spans="1:4">
-      <c r="A746" s="3"/>
-      <c r="B746" s="3"/>
-      <c r="C746" s="10"/>
-    </row>
-    <row r="747" spans="1:4">
-      <c r="A747" s="3"/>
-      <c r="B747" s="3"/>
-      <c r="C747" s="10"/>
-    </row>
-    <row r="748" spans="1:4">
-      <c r="A748" s="3"/>
-      <c r="B748" s="3"/>
-      <c r="C748" s="10"/>
-    </row>
-    <row r="749" spans="1:4">
-      <c r="A749" s="3"/>
-      <c r="B749" s="3"/>
-      <c r="C749" s="10"/>
-    </row>
-    <row r="750" spans="1:4">
-      <c r="A750" s="3"/>
-      <c r="B750" s="3"/>
-      <c r="C750" s="10"/>
-    </row>
-    <row r="751" spans="1:4">
-      <c r="A751" s="3"/>
-      <c r="B751" s="3"/>
-      <c r="C751" s="10"/>
-    </row>
-    <row r="752" spans="1:4">
-      <c r="A752" s="3"/>
-      <c r="B752" s="3"/>
-      <c r="C752" s="10"/>
-    </row>
-    <row r="753" spans="1:3">
-      <c r="A753" s="3"/>
-      <c r="B753" s="3"/>
-      <c r="C753" s="10"/>
-    </row>
-    <row r="754" spans="1:3">
-      <c r="A754" s="3"/>
-      <c r="B754" s="3"/>
-      <c r="C754" s="10"/>
-    </row>
-    <row r="755" spans="1:3">
-      <c r="A755" s="3"/>
-      <c r="B755" s="3"/>
-      <c r="C755" s="10"/>
-    </row>
-    <row r="756" spans="1:3">
-      <c r="A756" s="3"/>
-      <c r="B756" s="3"/>
-      <c r="C756" s="10"/>
-    </row>
-    <row r="757" spans="1:3">
-      <c r="A757" s="3"/>
-      <c r="B757" s="3"/>
-      <c r="C757" s="10"/>
-    </row>
-    <row r="758" spans="1:3">
-      <c r="A758" s="3"/>
-      <c r="B758" s="3"/>
-      <c r="C758" s="10"/>
-    </row>
-    <row r="759" spans="1:3">
-      <c r="A759" s="3"/>
-      <c r="B759" s="3"/>
-      <c r="C759" s="10"/>
-    </row>
-    <row r="760" spans="1:3">
-      <c r="A760" s="3"/>
-      <c r="B760" s="3"/>
-      <c r="C760" s="10"/>
-    </row>
-    <row r="761" spans="1:3">
-      <c r="A761" s="3"/>
-      <c r="B761" s="3"/>
-      <c r="C761" s="10"/>
-    </row>
-    <row r="762" spans="1:3">
-      <c r="A762" s="3"/>
-      <c r="B762" s="3"/>
-      <c r="C762" s="10"/>
-    </row>
-    <row r="763" spans="1:3">
-      <c r="A763" s="3"/>
-      <c r="B763" s="3"/>
-      <c r="C763" s="8"/>
-    </row>
-    <row r="764" spans="1:3">
-      <c r="A764" s="3"/>
-      <c r="B764" s="3"/>
-      <c r="C764" s="8"/>
-    </row>
-    <row r="765" spans="1:3">
-      <c r="B765" s="3"/>
-      <c r="C765" s="8"/>
-    </row>
-    <row r="766" spans="1:3">
-      <c r="B766" s="3"/>
-      <c r="C766" s="8"/>
-    </row>
-    <row r="767" spans="1:3">
-      <c r="B767" s="3"/>
-      <c r="C767" s="8"/>
-    </row>
-    <row r="768" spans="1:3">
-      <c r="B768" s="3"/>
-      <c r="C768" s="8"/>
+        <v>2425</v>
+      </c>
+      <c r="G743" t="s">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="744" spans="1:7">
+      <c r="A744" t="s">
+        <v>2393</v>
+      </c>
+      <c r="B744" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C744" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D744" t="s">
+        <v>2425</v>
+      </c>
+      <c r="G744" t="s">
+        <v>2496</v>
+      </c>
+    </row>
+    <row r="745" spans="1:7">
+      <c r="A745" t="s">
+        <v>2394</v>
+      </c>
+      <c r="B745" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C745" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D745" t="s">
+        <v>2425</v>
+      </c>
+      <c r="G745" t="s">
+        <v>2497</v>
+      </c>
+    </row>
+    <row r="746" spans="1:7">
+      <c r="A746" t="s">
+        <v>2395</v>
+      </c>
+      <c r="B746" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C746" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D746" t="s">
+        <v>2425</v>
+      </c>
+      <c r="G746" t="s">
+        <v>2498</v>
+      </c>
+    </row>
+    <row r="747" spans="1:7">
+      <c r="A747" t="s">
+        <v>2396</v>
+      </c>
+      <c r="B747" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C747" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D747" t="s">
+        <v>2425</v>
+      </c>
+      <c r="G747" t="s">
+        <v>2499</v>
+      </c>
+    </row>
+    <row r="748" spans="1:7">
+      <c r="A748" t="s">
+        <v>2397</v>
+      </c>
+      <c r="B748" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C748" s="14" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D748" t="s">
+        <v>2425</v>
+      </c>
+      <c r="G748" t="s">
+        <v>2500</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>